<commit_message>
Se corrigió los estilos de inventario y arqueo de caja
</commit_message>
<xml_diff>
--- a/Product_Backlog borrador.xlsx
+++ b/Product_Backlog borrador.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\USFX\CIENCIAS DE LA COMPUTACION\6to semestre\Arquitectura de software\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Arquitectura de software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94EA7E9-E0B8-4201-B159-C42B6D9D8DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22E830D-6E89-47AA-B4F3-CD1F51F2A5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,8 +35,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="82">
   <si>
     <t>Columna</t>
   </si>
@@ -217,9 +239,6 @@
     <t>H-8</t>
   </si>
   <si>
-    <t>Planificada</t>
-  </si>
-  <si>
     <t>Como administrador , quiero poder ver los ingresos y egresos de la cafetería, para poder tener control claro de las entradas registradas</t>
   </si>
   <si>
@@ -232,9 +251,6 @@
     <t>Sprint 3</t>
   </si>
   <si>
-    <t>Sprint 4</t>
-  </si>
-  <si>
     <t>Esta historia es fundamental para la operación de la cafetería, ya que permite que los cajeros registren los productos que los clientes consumen, agilizando el proceso de cobro y reduciendo tiempos de espera. Un sistema eficiente de registro contribuirá a evitar errores y mejorar la experiencia del cliente.</t>
   </si>
   <si>
@@ -257,13 +273,52 @@
   </si>
   <si>
     <t>Permite gestionar al personal de la cafetería, llevando control de horarios, roles y desempeño. Una buena implementación incluiría permisos de acceso diferenciados y reportes sobre el rendimiento del equipo.</t>
+  </si>
+  <si>
+    <t>H-9</t>
+  </si>
+  <si>
+    <t>En Proceso</t>
+  </si>
+  <si>
+    <t>H-10</t>
+  </si>
+  <si>
+    <t>H-11</t>
+  </si>
+  <si>
+    <t>Como cajero, quiero que se muestre un mensaje de confirmación al registrar los productos consumidos, para asegurarme de que la inserción se realizó correctamente.</t>
+  </si>
+  <si>
+    <t>Como cajero, quiero que las filas en la tabla de arqueo de caja tengan colores intercalados para facilitar la lectura y visualización de los datos.</t>
+  </si>
+  <si>
+    <t>Como cajero, quiero que el arqueo de caja muestre un desglose por denominaciones de billetes para facilitar el control de las ganancias diarias.</t>
+  </si>
+  <si>
+    <t>Se debe mostrar un mensaje de confirmación tras registrar un producto exitosamente.</t>
+  </si>
+  <si>
+    <t>Confirmación de registro de productos</t>
+  </si>
+  <si>
+    <t>Las filas de la tabla deben alternar colores de manera automática.</t>
+  </si>
+  <si>
+    <t>Intercalado de colores en arqueo de caja</t>
+  </si>
+  <si>
+    <t>La pantalla de arqueo de caja debe mostrar la cantidad total de dinero desglosada por denominaciones de billetes.</t>
+  </si>
+  <si>
+    <t>Desglose de billetes en arqueo de caja</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,13 +351,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -392,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -416,6 +464,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -425,24 +486,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -782,10 +827,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:L14"/>
+  <dimension ref="B1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="85" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -815,8 +860,9 @@
       <c r="B2" s="4"/>
     </row>
     <row r="4" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="6" t="s">
-        <v>2</v>
+      <c r="B4" s="6" t="e" cm="1">
+        <f t="array" ref="B4">B4:I14Identificador (ID) de la Historia</f>
+        <v>#NAME?</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>3</v>
@@ -863,7 +909,7 @@
         <v>39</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="G5" s="10">
         <v>8</v>
@@ -872,17 +918,17 @@
         <v>3</v>
       </c>
       <c r="I5" s="10">
-        <f t="shared" ref="I5:I12" si="0">G5/H5</f>
+        <f t="shared" ref="I5:I15" si="0">G5/H5</f>
         <v>2.6666666666666665</v>
       </c>
-      <c r="J5" s="11" t="s">
-        <v>59</v>
+      <c r="J5" s="16" t="s">
+        <v>58</v>
       </c>
       <c r="K5" s="9">
         <v>1</v>
       </c>
-      <c r="L5" s="20" t="s">
-        <v>63</v>
+      <c r="L5" s="11" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
@@ -899,7 +945,7 @@
         <v>40</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="G6" s="10">
         <v>6</v>
@@ -911,12 +957,12 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="J6" s="12"/>
+      <c r="J6" s="17"/>
       <c r="K6" s="9">
         <v>2</v>
       </c>
-      <c r="L6" s="20" t="s">
-        <v>64</v>
+      <c r="L6" s="11" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
@@ -933,77 +979,77 @@
         <v>47</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="G7" s="10">
         <v>9</v>
       </c>
       <c r="H7" s="10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I7" s="10">
         <f t="shared" si="0"/>
-        <v>1.8</v>
-      </c>
-      <c r="J7" s="13"/>
+        <v>1.5</v>
+      </c>
+      <c r="J7" s="18"/>
       <c r="K7" s="9">
         <v>3</v>
       </c>
-      <c r="L7" s="20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>46</v>
+      <c r="L7" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B8" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>81</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="G8" s="10">
-        <v>7</v>
-      </c>
-      <c r="H8" s="10">
+        <v>70</v>
+      </c>
+      <c r="G8" s="14">
+        <v>9</v>
+      </c>
+      <c r="H8" s="14">
         <v>5</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="14">
         <f t="shared" si="0"/>
-        <v>1.4</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>60</v>
+        <v>1.8</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>59</v>
       </c>
       <c r="K8" s="9">
         <v>4</v>
       </c>
-      <c r="L8" s="20" t="s">
-        <v>66</v>
+      <c r="L8" s="11" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>35</v>
+        <v>57</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="G9" s="10">
         <v>7</v>
@@ -1015,65 +1061,63 @@
         <f t="shared" si="0"/>
         <v>1.4</v>
       </c>
-      <c r="J9" s="13"/>
+      <c r="J9" s="17"/>
       <c r="K9" s="9">
         <v>5</v>
       </c>
-      <c r="L9" s="20" t="s">
-        <v>67</v>
+      <c r="L9" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="G10" s="10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H10" s="10">
         <v>5</v>
       </c>
       <c r="I10" s="10">
         <f t="shared" si="0"/>
-        <v>1.2</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>61</v>
-      </c>
+        <v>1.4</v>
+      </c>
+      <c r="J10" s="18"/>
       <c r="K10" s="9">
         <v>6</v>
       </c>
-      <c r="L10" s="20" t="s">
-        <v>68</v>
+      <c r="L10" s="11" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="G11" s="10">
         <v>6</v>
@@ -1085,84 +1129,201 @@
         <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
-      <c r="J11" s="13"/>
+      <c r="J11" s="19" t="s">
+        <v>60</v>
+      </c>
       <c r="K11" s="9">
         <v>7</v>
       </c>
-      <c r="L11" s="20" t="s">
-        <v>69</v>
+      <c r="L11" s="11" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="G12" s="10">
+        <v>6</v>
+      </c>
+      <c r="H12" s="10">
         <v>5</v>
-      </c>
-      <c r="H12" s="10">
-        <v>12</v>
       </c>
       <c r="I12" s="10">
         <f t="shared" si="0"/>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>62</v>
-      </c>
+        <v>1.2</v>
+      </c>
+      <c r="J12" s="19"/>
       <c r="K12" s="9">
         <v>8</v>
       </c>
-      <c r="L12" s="20" t="s">
+      <c r="L12" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="8"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="17"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="17"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="8"/>
+      <c r="G13" s="10">
+        <v>5</v>
+      </c>
+      <c r="H13" s="10">
+        <v>12</v>
+      </c>
+      <c r="I13" s="10">
+        <f t="shared" si="0"/>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="J13" s="19"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="13"/>
+    </row>
+    <row r="14" spans="2:12" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="14">
+        <v>7</v>
+      </c>
+      <c r="H14" s="14">
+        <v>30</v>
+      </c>
+      <c r="I14" s="10">
+        <f t="shared" si="0"/>
+        <v>0.23333333333333334</v>
+      </c>
       <c r="J14" s="17"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="17"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="13"/>
+    </row>
+    <row r="15" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B15" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="14">
+        <v>5</v>
+      </c>
+      <c r="H15" s="14">
+        <v>30</v>
+      </c>
+      <c r="I15" s="10">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="J15" s="18"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:I14">
-    <sortCondition descending="1" ref="I5:I14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:I15">
+    <sortCondition descending="1" ref="I5:I15"/>
   </sortState>
-  <mergeCells count="3">
+  <mergeCells count="4">
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="J14:J15"/>
     <mergeCell ref="J5:J7"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="J8:J10"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -1174,8 +1335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>